<commit_message>
Trying to get graphs
</commit_message>
<xml_diff>
--- a/randomized_search_cvWHITE.xlsx
+++ b/randomized_search_cvWHITE.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziecarey/Documents/Wine_Regression/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-500" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="randomized_search_cvWHITE" sheetId="1" r:id="rId1"/>
@@ -186,7 +181,17 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US" baseline="0"/>
           </a:p>
@@ -201,26 +206,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -253,6 +238,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>randomized_search_cvWHITE!$A$1:$A$10</c:f>
@@ -341,11 +332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2088733696"/>
-        <c:axId val="-2088446928"/>
+        <c:axId val="2075608200"/>
+        <c:axId val="2075612024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2088733696"/>
+        <c:axId val="2075608200"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -401,26 +392,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -459,12 +430,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088446928"/>
+        <c:crossAx val="2075612024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2088446928"/>
+        <c:axId val="2075612024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,26 +490,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -577,7 +528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088733696"/>
+        <c:crossAx val="2075608200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -679,26 +630,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -946,11 +877,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2117789648"/>
-        <c:axId val="-2083273712"/>
+        <c:axId val="2075678712"/>
+        <c:axId val="2075687528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2117789648"/>
+        <c:axId val="2075678712"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1006,26 +937,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -1064,12 +975,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083273712"/>
+        <c:crossAx val="2075687528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2083273712"/>
+        <c:axId val="2075687528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,26 +1035,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1182,7 +1073,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117789648"/>
+        <c:crossAx val="2075678712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2483,7 +2374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2518,7 +2409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2695,7 +2586,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2706,12 +2597,12 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1">
         <v>1.0000000000000099E-6</v>
       </c>
@@ -2725,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1.00019999999999E-5</v>
       </c>
@@ -2739,7 +2630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1.0002000400000001E-4</v>
       </c>
@@ -2753,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1.0002000400080001E-3</v>
       </c>
@@ -2767,7 +2658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>1.00020004000798E-2</v>
       </c>
@@ -2781,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>0.10002000400080099</v>
       </c>
@@ -2795,7 +2686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1.000200040008</v>
       </c>
@@ -2809,7 +2700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>10.00200040008</v>
       </c>
@@ -2823,7 +2714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>100.0200040008</v>
       </c>
@@ -2837,7 +2728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1000.200040008</v>
       </c>
@@ -2851,7 +2742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -2859,7 +2750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1.0000000000000099E-6</v>
       </c>
@@ -2870,7 +2761,7 @@
         <v>0.51223483000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>1.00019999999999E-5</v>
       </c>
@@ -2881,7 +2772,7 @@
         <v>0.51327794999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>1.0002000400000001E-4</v>
       </c>
@@ -2892,7 +2783,7 @@
         <v>0.51346455000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>1.0002000400080001E-3</v>
       </c>
@@ -2903,7 +2794,7 @@
         <v>0.51547520999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>1.00020004000798E-2</v>
       </c>
@@ -2914,7 +2805,7 @@
         <v>0.52725988999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>0.10002000400080099</v>
       </c>
@@ -2925,7 +2816,7 @@
         <v>0.56184811999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1.000200040008</v>
       </c>
@@ -2936,7 +2827,7 @@
         <v>0.60886048000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>10.00200040008</v>
       </c>
@@ -2947,7 +2838,7 @@
         <v>0.63288840000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>100.0200040008</v>
       </c>
@@ -2958,7 +2849,7 @@
         <v>0.64855103999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>1000.200040008</v>
       </c>
@@ -2972,5 +2863,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>